<commit_message>
Measure best time. Better CSV formatting for output results
</commit_message>
<xml_diff>
--- a/docs/orders-performance.xlsx
+++ b/docs/orders-performance.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="31">
   <si>
     <t xml:space="preserve">Job </t>
   </si>
@@ -59,27 +59,12 @@
     <t>PING</t>
   </si>
   <si>
-    <t>percentiles[ms] 50th</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> execution time[s]</t>
-  </si>
-  <si>
     <t>IOPS</t>
   </si>
   <si>
     <t>Total job time[s]</t>
   </si>
   <si>
-    <t>Threads</t>
-  </si>
-  <si>
-    <t>Iterations per thread</t>
-  </si>
-  <si>
-    <t>Total requests sent</t>
-  </si>
-  <si>
     <t>NEWCUSTOMER</t>
   </si>
   <si>
@@ -104,9 +89,6 @@
     <t>Database</t>
   </si>
   <si>
-    <t>MySQL</t>
-  </si>
-  <si>
     <t>HTTP server</t>
   </si>
   <si>
@@ -122,18 +104,36 @@
     <t>Server JVM options</t>
   </si>
   <si>
-    <t>Total # of GC: 7</t>
-  </si>
-  <si>
-    <t>Total GC Time (ms): 57</t>
+    <t>MySQL 5.7.19 with Docker</t>
+  </si>
+  <si>
+    <t>PINGS_STREAM</t>
+  </si>
+  <si>
+    <t>Operation</t>
+  </si>
+  <si>
+    <t>Tomcat 8.5.16</t>
+  </si>
+  <si>
+    <t>-Xmx500m</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -162,11 +162,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -447,29 +452,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB28"/>
+  <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
     <col min="10" max="10" width="4.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
         <v>26</v>
@@ -477,66 +483,72 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:15" s="1" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F7" s="1" t="s">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="M7" s="1" t="s">
+      <c r="J7" s="2"/>
+      <c r="K7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N7" s="1" t="s">
+      <c r="N7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="O7" s="1" t="s">
+      <c r="O7" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
         <v>0</v>
@@ -577,7 +589,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
@@ -621,7 +633,7 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
@@ -665,13 +677,13 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D11">
         <v>8.5259999999999998</v>
@@ -709,7 +721,7 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B14" t="s">
         <v>9</v>
@@ -753,7 +765,7 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
         <v>9</v>
@@ -797,7 +809,7 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
         <v>9</v>
@@ -839,15 +851,15 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
         <v>9</v>
       </c>
       <c r="C17" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D17">
         <v>8.9160000000000004</v>
@@ -883,9 +895,9 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B19" t="s">
         <v>0</v>
@@ -924,9 +936,9 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B20" t="s">
         <v>0</v>
@@ -968,134 +980,220 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21">
+        <v>0.55900000000000005</v>
+      </c>
+      <c r="E21">
+        <v>1.294</v>
+      </c>
+      <c r="F21">
+        <v>2.2370000000000001</v>
+      </c>
+      <c r="G21">
+        <v>6.032</v>
+      </c>
+      <c r="H21">
+        <v>78.366</v>
+      </c>
+      <c r="I21">
+        <v>144.648</v>
+      </c>
+      <c r="K21">
+        <v>1617</v>
+      </c>
+      <c r="L21">
+        <v>32.584000000000003</v>
+      </c>
+      <c r="M21">
+        <v>1</v>
+      </c>
+      <c r="N21">
+        <v>50000</v>
+      </c>
+      <c r="O21">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22">
+        <v>9.4529999999999994</v>
+      </c>
+      <c r="E22">
+        <v>17.324000000000002</v>
+      </c>
+      <c r="F22">
+        <v>30.341999999999999</v>
+      </c>
+      <c r="G22">
+        <v>57.232999999999997</v>
+      </c>
+      <c r="H22">
+        <v>77.427999999999997</v>
+      </c>
+      <c r="I22">
+        <v>78.808999999999997</v>
+      </c>
+      <c r="K22">
+        <v>101</v>
+      </c>
+      <c r="L22">
+        <v>298.23599999999999</v>
+      </c>
+      <c r="M22">
+        <v>1</v>
+      </c>
+      <c r="N22">
+        <v>30000</v>
+      </c>
+      <c r="O22">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B28" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>15</v>
+      </c>
+      <c r="B32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32">
+        <v>1.2849999999999999</v>
+      </c>
+      <c r="E32">
+        <v>6.1920000000000002</v>
+      </c>
+      <c r="F32">
+        <v>12.395</v>
+      </c>
+      <c r="G32">
+        <v>25.603000000000002</v>
+      </c>
+      <c r="H32">
+        <v>34.438000000000002</v>
+      </c>
+      <c r="I32">
+        <v>35.42</v>
+      </c>
+      <c r="K32">
+        <v>655</v>
+      </c>
+      <c r="L32">
+        <v>9.077</v>
+      </c>
+      <c r="M32">
+        <v>1</v>
+      </c>
+      <c r="N32">
+        <v>5000</v>
+      </c>
+      <c r="O32">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>15</v>
+      </c>
+      <c r="B33" t="s">
         <v>9</v>
       </c>
-      <c r="C21" t="s">
-        <v>18</v>
-      </c>
-      <c r="D21">
-        <v>9.4529999999999994</v>
-      </c>
-      <c r="E21">
-        <v>17.324000000000002</v>
-      </c>
-      <c r="F21">
-        <v>30.341999999999999</v>
-      </c>
-      <c r="G21">
-        <v>57.232999999999997</v>
-      </c>
-      <c r="H21">
-        <v>77.427999999999997</v>
-      </c>
-      <c r="I21">
-        <v>78.808999999999997</v>
-      </c>
-      <c r="K21">
-        <v>101</v>
-      </c>
-      <c r="L21">
-        <v>298.23599999999999</v>
-      </c>
-      <c r="M21">
-        <v>1</v>
-      </c>
-      <c r="N21">
-        <v>30000</v>
-      </c>
-      <c r="O21">
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>9</v>
-      </c>
-      <c r="B28" t="s">
+      <c r="C33" t="s">
         <v>10</v>
       </c>
-      <c r="C28" t="s">
-        <v>11</v>
-      </c>
-      <c r="D28">
-        <v>0.75800000000000001</v>
-      </c>
-      <c r="E28" t="s">
-        <v>1</v>
-      </c>
-      <c r="F28">
-        <v>2.2509999999999999</v>
-      </c>
-      <c r="G28" t="s">
-        <v>2</v>
-      </c>
-      <c r="H28">
-        <v>4.6310000000000002</v>
-      </c>
-      <c r="I28" t="s">
-        <v>3</v>
-      </c>
-      <c r="J28">
-        <v>10.444000000000001</v>
-      </c>
-      <c r="K28" t="s">
-        <v>4</v>
-      </c>
-      <c r="L28">
-        <v>22.882999999999999</v>
-      </c>
-      <c r="M28" t="s">
-        <v>5</v>
-      </c>
-      <c r="N28">
-        <v>28.707000000000001</v>
-      </c>
-      <c r="O28" t="s">
-        <v>12</v>
-      </c>
-      <c r="P28">
-        <v>41.988</v>
-      </c>
-      <c r="Q28" t="s">
-        <v>13</v>
-      </c>
-      <c r="R28">
-        <v>1191</v>
-      </c>
-      <c r="S28" t="s">
-        <v>14</v>
-      </c>
-      <c r="T28">
-        <v>43.862000000000002</v>
-      </c>
-      <c r="U28" t="s">
-        <v>15</v>
-      </c>
-      <c r="V28">
-        <v>1</v>
-      </c>
-      <c r="W28" t="s">
-        <v>16</v>
-      </c>
-      <c r="X28">
+      <c r="D33">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="E33">
+        <v>4.2759999999999998</v>
+      </c>
+      <c r="F33">
+        <v>6.4349999999999996</v>
+      </c>
+      <c r="G33">
+        <v>12.582000000000001</v>
+      </c>
+      <c r="H33">
+        <v>26.832000000000001</v>
+      </c>
+      <c r="I33">
+        <v>32.9</v>
+      </c>
+      <c r="K33">
+        <v>896</v>
+      </c>
+      <c r="L33">
+        <v>56.947000000000003</v>
+      </c>
+      <c r="M33">
+        <v>1</v>
+      </c>
+      <c r="N33">
         <v>50000</v>
       </c>
-      <c r="Y28" t="s">
-        <v>17</v>
-      </c>
-      <c r="Z28">
+      <c r="O33">
         <v>50000</v>
-      </c>
-      <c r="AA28" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB28" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CSV formatting for performance metrics. Remove service discovery and configuration services from orders projects. Linux scripts for tests
</commit_message>
<xml_diff>
--- a/docs/orders-performance.xlsx
+++ b/docs/orders-performance.xlsx
@@ -15,6 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="37">
   <si>
     <t xml:space="preserve">Job </t>
   </si>
@@ -62,9 +63,6 @@
     <t>IOPS</t>
   </si>
   <si>
-    <t>Total job time[s]</t>
-  </si>
-  <si>
     <t>NEWCUSTOMER</t>
   </si>
   <si>
@@ -117,12 +115,37 @@
   </si>
   <si>
     <t>-Xmx500m</t>
+  </si>
+  <si>
+    <t>0th</t>
+  </si>
+  <si>
+    <t>Orders-HTTP-Client</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Orders-gRPC-Client</t>
+  </si>
+  <si>
+    <t>execution time [s]</t>
+  </si>
+  <si>
+    <t>Total job time [s]</t>
+  </si>
+  <si>
+    <t>Orders-HTTPS-Client</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -162,7 +185,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -172,6 +195,8 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -452,103 +477,112 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O33"/>
+  <dimension ref="A1:P42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
     <col min="3" max="3" width="16.85546875" customWidth="1"/>
-    <col min="10" max="10" width="4.28515625" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" customWidth="1"/>
+    <col min="11" max="11" width="9.85546875" customWidth="1"/>
+    <col min="12" max="12" width="11" customWidth="1"/>
+    <col min="13" max="13" width="11.7109375" customWidth="1"/>
+    <col min="15" max="15" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" s="1" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" s="1" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="F7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="I7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="J7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J7" s="2"/>
       <c r="K7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="L7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L7" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="M7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N7" s="2" t="s">
+      <c r="O7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="O7" s="2" t="s">
+      <c r="P7" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
         <v>0</v>
@@ -556,40 +590,40 @@
       <c r="C8" t="s">
         <v>10</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>0.77100000000000002</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>1.7130000000000001</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>2.5659999999999998</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>6.4969999999999999</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>45.670999999999999</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>62.228999999999999</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>1104</v>
       </c>
-      <c r="M8">
-        <v>1</v>
-      </c>
       <c r="N8">
-        <v>30000</v>
+        <v>1</v>
       </c>
       <c r="O8">
         <v>30000</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P8">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
@@ -597,43 +631,43 @@
       <c r="C9" t="s">
         <v>10</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>0.79700000000000004</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>1.6439999999999999</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>3.319</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>7.06</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>16.077999999999999</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>18.074000000000002</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>1145</v>
       </c>
-      <c r="L9">
+      <c r="M9" s="6">
         <v>18.545000000000002</v>
       </c>
-      <c r="M9">
-        <v>1</v>
-      </c>
       <c r="N9">
-        <v>20000</v>
+        <v>1</v>
       </c>
       <c r="O9">
         <v>20000</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P9">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
@@ -641,87 +675,93 @@
       <c r="C10" t="s">
         <v>10</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>1.3080000000000001</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>2.19</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>3.17</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>7.2960000000000003</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>15.456</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>15.984999999999999</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>724</v>
       </c>
-      <c r="L10">
+      <c r="M10" s="6">
         <v>70.665000000000006</v>
       </c>
-      <c r="M10">
-        <v>1</v>
-      </c>
       <c r="N10">
-        <v>50000</v>
+        <v>1</v>
       </c>
       <c r="O10">
         <v>50000</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P10">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11">
+        <v>12</v>
+      </c>
+      <c r="E11">
         <v>8.5259999999999998</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>16.792999999999999</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>28.111999999999998</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>36.161000000000001</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>39.887</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>40.301000000000002</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <v>114</v>
       </c>
-      <c r="L11">
+      <c r="M11" s="6">
         <v>45.545000000000002</v>
       </c>
-      <c r="M11">
-        <v>1</v>
-      </c>
       <c r="N11">
-        <v>5000</v>
+        <v>1</v>
       </c>
       <c r="O11">
         <v>5000</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P11">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M12" s="6"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M13" s="6"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
         <v>9</v>
@@ -729,43 +769,43 @@
       <c r="C14" t="s">
         <v>10</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <v>1.075</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>2.2759999999999998</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>3.161</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>8.3580000000000005</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>172.42500000000001</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>205.40100000000001</v>
       </c>
-      <c r="K14">
+      <c r="L14">
         <v>846</v>
       </c>
-      <c r="L14">
+      <c r="M14" s="6">
         <v>36.341000000000001</v>
       </c>
-      <c r="M14">
-        <v>1</v>
-      </c>
       <c r="N14">
-        <v>30000</v>
+        <v>1</v>
       </c>
       <c r="O14">
         <v>30000</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P14">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
         <v>9</v>
@@ -773,43 +813,43 @@
       <c r="C15" t="s">
         <v>10</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>1.0409999999999999</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>1.756</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>2.9079999999999999</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>7.6429999999999998</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>10.54</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>11.635999999999999</v>
       </c>
-      <c r="K15">
+      <c r="L15">
         <v>926</v>
       </c>
-      <c r="L15">
+      <c r="M15" s="6">
         <v>55.301000000000002</v>
       </c>
-      <c r="M15">
-        <v>1</v>
-      </c>
       <c r="N15">
-        <v>50000</v>
+        <v>1</v>
       </c>
       <c r="O15">
         <v>50000</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P15">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
         <v>9</v>
@@ -817,87 +857,90 @@
       <c r="C16" t="s">
         <v>10</v>
       </c>
-      <c r="D16">
+      <c r="E16">
         <v>1.0389999999999999</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>1.74</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>2.7280000000000002</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>7.7279999999999998</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <v>13.301</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <v>14.773</v>
       </c>
-      <c r="K16">
+      <c r="L16">
         <v>927</v>
       </c>
-      <c r="L16">
+      <c r="M16" s="6">
         <v>55.267000000000003</v>
       </c>
-      <c r="M16">
-        <v>1</v>
-      </c>
       <c r="N16">
-        <v>50000</v>
+        <v>1</v>
       </c>
       <c r="O16">
         <v>50000</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P16">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" t="s">
         <v>9</v>
       </c>
       <c r="C17" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17">
+        <v>12</v>
+      </c>
+      <c r="E17">
         <v>8.9160000000000004</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>17.009</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>32.76</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>50.883000000000003</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <v>55.804000000000002</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <v>55.941000000000003</v>
       </c>
-      <c r="K17">
+      <c r="L17">
         <v>110</v>
       </c>
-      <c r="L17">
+      <c r="M17" s="6">
         <v>185.083</v>
       </c>
-      <c r="M17">
-        <v>1</v>
-      </c>
       <c r="N17">
-        <v>20000</v>
+        <v>1</v>
       </c>
       <c r="O17">
         <v>20000</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P17">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M18" s="6"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B19" t="s">
         <v>0</v>
@@ -905,40 +948,41 @@
       <c r="C19" t="s">
         <v>10</v>
       </c>
-      <c r="D19">
+      <c r="E19">
         <v>0.68</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <v>2.39</v>
       </c>
-      <c r="F19">
+      <c r="G19">
         <v>4.6829999999999998</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <v>13.452</v>
       </c>
-      <c r="H19">
+      <c r="I19">
         <v>385.96499999999997</v>
       </c>
-      <c r="I19">
+      <c r="J19">
         <v>543.07299999999998</v>
       </c>
-      <c r="K19">
+      <c r="L19">
         <v>1179</v>
       </c>
-      <c r="M19">
-        <v>1</v>
-      </c>
+      <c r="M19" s="6"/>
       <c r="N19">
-        <v>30000</v>
+        <v>1</v>
       </c>
       <c r="O19">
         <v>30000</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P19">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B20" t="s">
         <v>0</v>
@@ -946,253 +990,496 @@
       <c r="C20" t="s">
         <v>10</v>
       </c>
-      <c r="D20">
+      <c r="E20">
         <v>0.75800000000000001</v>
       </c>
-      <c r="E20">
+      <c r="F20">
         <v>2.2509999999999999</v>
       </c>
-      <c r="F20">
+      <c r="G20">
         <v>4.6310000000000002</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <v>10.444000000000001</v>
       </c>
-      <c r="H20">
+      <c r="I20">
         <v>22.882999999999999</v>
       </c>
-      <c r="I20">
+      <c r="J20">
         <v>28.707000000000001</v>
       </c>
-      <c r="K20">
+      <c r="L20">
         <v>1191</v>
       </c>
-      <c r="L20">
+      <c r="M20" s="6">
         <v>43.862000000000002</v>
       </c>
-      <c r="M20">
-        <v>1</v>
-      </c>
       <c r="N20">
-        <v>50000</v>
+        <v>1</v>
       </c>
       <c r="O20">
         <v>50000</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P20">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B21" t="s">
         <v>0</v>
       </c>
       <c r="C21" t="s">
-        <v>27</v>
-      </c>
-      <c r="D21">
+        <v>26</v>
+      </c>
+      <c r="E21">
         <v>0.55900000000000005</v>
       </c>
-      <c r="E21">
+      <c r="F21">
         <v>1.294</v>
       </c>
-      <c r="F21">
+      <c r="G21">
         <v>2.2370000000000001</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <v>6.032</v>
       </c>
-      <c r="H21">
+      <c r="I21">
         <v>78.366</v>
       </c>
-      <c r="I21">
+      <c r="J21">
         <v>144.648</v>
       </c>
-      <c r="K21">
+      <c r="L21">
         <v>1617</v>
       </c>
-      <c r="L21">
+      <c r="M21" s="6">
         <v>32.584000000000003</v>
       </c>
-      <c r="M21">
-        <v>1</v>
-      </c>
       <c r="N21">
-        <v>50000</v>
+        <v>1</v>
       </c>
       <c r="O21">
         <v>50000</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P21">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B22" t="s">
         <v>9</v>
       </c>
       <c r="C22" t="s">
-        <v>13</v>
-      </c>
-      <c r="D22">
+        <v>12</v>
+      </c>
+      <c r="E22">
         <v>9.4529999999999994</v>
       </c>
-      <c r="E22">
+      <c r="F22">
         <v>17.324000000000002</v>
       </c>
-      <c r="F22">
+      <c r="G22">
         <v>30.341999999999999</v>
       </c>
-      <c r="G22">
+      <c r="H22">
         <v>57.232999999999997</v>
       </c>
-      <c r="H22">
+      <c r="I22">
         <v>77.427999999999997</v>
       </c>
-      <c r="I22">
+      <c r="J22">
         <v>78.808999999999997</v>
       </c>
-      <c r="K22">
+      <c r="L22">
         <v>101</v>
       </c>
-      <c r="L22">
+      <c r="M22" s="6">
         <v>298.23599999999999</v>
       </c>
-      <c r="M22">
-        <v>1</v>
-      </c>
       <c r="N22">
-        <v>30000</v>
+        <v>1</v>
       </c>
       <c r="O22">
         <v>30000</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P22">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M23" s="6"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" t="s">
+        <v>32</v>
+      </c>
+      <c r="D30" s="5">
+        <v>0.52600000000000002</v>
+      </c>
+      <c r="E30" s="5">
+        <v>0.73</v>
+      </c>
+      <c r="F30" s="5">
+        <v>1.8180000000000001</v>
+      </c>
+      <c r="G30" s="5">
+        <v>4.9729999999999999</v>
+      </c>
+      <c r="H30" s="5">
+        <v>11.02</v>
+      </c>
+      <c r="I30" s="5">
+        <v>19.125</v>
+      </c>
+      <c r="J30" s="5">
+        <v>20.643999999999998</v>
+      </c>
+      <c r="K30" s="6">
+        <v>25.202000000000002</v>
+      </c>
+      <c r="L30" s="6">
+        <v>1190.3820000000001</v>
+      </c>
+      <c r="M30" s="6">
+        <v>26.221</v>
+      </c>
+      <c r="N30">
+        <v>1</v>
+      </c>
+      <c r="O30">
+        <v>30000</v>
+      </c>
+      <c r="P30">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" t="s">
+        <v>10</v>
+      </c>
+      <c r="C31" t="s">
+        <v>32</v>
+      </c>
+      <c r="D31" s="5">
+        <v>0.42799999999999999</v>
+      </c>
+      <c r="E31" s="5">
+        <v>0.66900000000000004</v>
+      </c>
+      <c r="F31" s="5">
+        <v>2.3769999999999998</v>
+      </c>
+      <c r="G31" s="5">
+        <v>4.5780000000000003</v>
+      </c>
+      <c r="H31" s="5">
+        <v>13.928000000000001</v>
+      </c>
+      <c r="I31" s="5">
+        <v>14.909000000000001</v>
+      </c>
+      <c r="J31" s="5">
+        <v>14.971</v>
+      </c>
+      <c r="K31" s="6">
+        <v>23.173999999999999</v>
+      </c>
+      <c r="L31" s="6">
+        <v>1294.6099999999999</v>
+      </c>
+      <c r="M31" s="6">
+        <v>24.936</v>
+      </c>
+      <c r="N31">
+        <v>1</v>
+      </c>
+      <c r="O31">
+        <v>30000</v>
+      </c>
+      <c r="P31">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" t="s">
+        <v>32</v>
+      </c>
+      <c r="D32">
+        <v>0.40899999999999997</v>
+      </c>
+      <c r="E32">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="F32">
+        <v>1.756</v>
+      </c>
+      <c r="G32">
+        <v>3.4140000000000001</v>
+      </c>
+      <c r="H32">
+        <v>10.909000000000001</v>
+      </c>
+      <c r="I32">
+        <v>16.245999999999999</v>
+      </c>
+      <c r="J32">
+        <v>17.878</v>
+      </c>
+      <c r="K32" s="6">
+        <v>34.335000000000001</v>
+      </c>
+      <c r="L32" s="6">
+        <v>1456.24</v>
+      </c>
+      <c r="M32" s="6">
+        <v>35.783999999999999</v>
+      </c>
+      <c r="N32">
+        <v>1</v>
+      </c>
+      <c r="O32">
+        <v>50000</v>
+      </c>
+      <c r="P32">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" t="s">
+        <v>32</v>
+      </c>
+      <c r="D33" s="5">
+        <v>0.66</v>
+      </c>
+      <c r="E33" s="5">
+        <v>0.97099999999999997</v>
+      </c>
+      <c r="F33" s="5">
+        <v>1.643</v>
+      </c>
+      <c r="G33" s="5">
+        <v>3.9350000000000001</v>
+      </c>
+      <c r="H33" s="5">
+        <v>6.0919999999999996</v>
+      </c>
+      <c r="I33" s="5">
+        <v>9.08</v>
+      </c>
+      <c r="J33" s="5">
+        <v>11.368</v>
+      </c>
+      <c r="K33" s="6">
+        <v>49.738999999999997</v>
+      </c>
+      <c r="L33" s="6">
+        <v>1005.247</v>
+      </c>
+      <c r="M33" s="6">
+        <v>50.84</v>
+      </c>
+      <c r="N33">
+        <v>1</v>
+      </c>
+      <c r="O33">
+        <v>50000</v>
+      </c>
+      <c r="P33">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B26" s="3" t="s">
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+      <c r="B36" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B27" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B28" s="3" t="s">
+      <c r="B37" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B39" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>15</v>
-      </c>
-      <c r="B32" t="s">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>14</v>
+      </c>
+      <c r="B41" t="s">
         <v>0</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C41" t="s">
         <v>10</v>
       </c>
-      <c r="D32">
+      <c r="E41">
         <v>1.2849999999999999</v>
       </c>
-      <c r="E32">
+      <c r="F41">
         <v>6.1920000000000002</v>
       </c>
-      <c r="F32">
+      <c r="G41">
         <v>12.395</v>
       </c>
-      <c r="G32">
+      <c r="H41">
         <v>25.603000000000002</v>
       </c>
-      <c r="H32">
+      <c r="I41">
         <v>34.438000000000002</v>
       </c>
-      <c r="I32">
+      <c r="J41">
         <v>35.42</v>
       </c>
-      <c r="K32">
+      <c r="L41">
         <v>655</v>
       </c>
-      <c r="L32">
+      <c r="M41">
         <v>9.077</v>
       </c>
-      <c r="M32">
-        <v>1</v>
-      </c>
-      <c r="N32">
+      <c r="N41">
+        <v>1</v>
+      </c>
+      <c r="O41">
         <v>5000</v>
       </c>
-      <c r="O32">
+      <c r="P41">
         <v>5000</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>15</v>
-      </c>
-      <c r="B33" t="s">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>14</v>
+      </c>
+      <c r="B42" t="s">
         <v>9</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C42" t="s">
         <v>10</v>
       </c>
-      <c r="D33">
+      <c r="E42">
         <v>0.98899999999999999</v>
       </c>
-      <c r="E33">
+      <c r="F42">
         <v>4.2759999999999998</v>
       </c>
-      <c r="F33">
+      <c r="G42">
         <v>6.4349999999999996</v>
       </c>
-      <c r="G33">
+      <c r="H42">
         <v>12.582000000000001</v>
       </c>
-      <c r="H33">
+      <c r="I42">
         <v>26.832000000000001</v>
       </c>
-      <c r="I33">
+      <c r="J42">
         <v>32.9</v>
       </c>
-      <c r="K33">
+      <c r="L42">
         <v>896</v>
       </c>
-      <c r="L33">
+      <c r="M42">
         <v>56.947000000000003</v>
       </c>
-      <c r="M33">
-        <v>1</v>
-      </c>
-      <c r="N33">
-        <v>50000</v>
-      </c>
-      <c r="O33">
+      <c r="N42">
+        <v>1</v>
+      </c>
+      <c r="O42">
+        <v>50000</v>
+      </c>
+      <c r="P42">
         <v>50000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Clean scripts for tests. Add performance results from corporate cloud and AWS
</commit_message>
<xml_diff>
--- a/docs/orders-performance.xlsx
+++ b/docs/orders-performance.xlsx
@@ -15,7 +15,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="218">
   <si>
     <t xml:space="preserve">Job </t>
   </si>
@@ -33,15 +32,6 @@
     <t xml:space="preserve"> 99th</t>
   </si>
   <si>
-    <t xml:space="preserve"> 99.9th</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 99.99th</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 99.999th</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 100th</t>
   </si>
   <si>
@@ -66,12 +56,6 @@
     <t>NEWCUSTOMER</t>
   </si>
   <si>
-    <t>HTTP 1.1</t>
-  </si>
-  <si>
-    <t>HTTPS 1.1</t>
-  </si>
-  <si>
     <t>gRPC + HTTP 2</t>
   </si>
   <si>
@@ -102,18 +86,12 @@
     <t>Server JVM options</t>
   </si>
   <si>
-    <t>MySQL 5.7.19 with Docker</t>
-  </si>
-  <si>
     <t>PINGS_STREAM</t>
   </si>
   <si>
     <t>Operation</t>
   </si>
   <si>
-    <t>Tomcat 8.5.16</t>
-  </si>
-  <si>
     <t>-Xmx500m</t>
   </si>
   <si>
@@ -136,6 +114,570 @@
   </si>
   <si>
     <t>Orders-HTTPS-Client</t>
+  </si>
+  <si>
+    <t>H2 in file</t>
+  </si>
+  <si>
+    <t>Server</t>
+  </si>
+  <si>
+    <t>EPAM cloud, SMALL, 1x Core, SSD, CentOS 7 64</t>
+  </si>
+  <si>
+    <t>Client</t>
+  </si>
+  <si>
+    <t>Client JVM options</t>
+  </si>
+  <si>
+    <t>-Xmx1g</t>
+  </si>
+  <si>
+    <t>50000.000</t>
+  </si>
+  <si>
+    <t>5.000</t>
+  </si>
+  <si>
+    <t>250000.000</t>
+  </si>
+  <si>
+    <t>10.000</t>
+  </si>
+  <si>
+    <t>30000.000</t>
+  </si>
+  <si>
+    <t>500000.000</t>
+  </si>
+  <si>
+    <t>Client server latency</t>
+  </si>
+  <si>
+    <t>MySQL 5,7,19 with Docker</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 99,9th</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 99,99th</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 99,999th</t>
+  </si>
+  <si>
+    <t>HTTP 1,1</t>
+  </si>
+  <si>
+    <t>HTTPS 1,1</t>
+  </si>
+  <si>
+    <t>Tomcat 8,5,16</t>
+  </si>
+  <si>
+    <t>min 0,4 ms, avg 0,6 ms</t>
+  </si>
+  <si>
+    <t>0.213</t>
+  </si>
+  <si>
+    <t>0.374</t>
+  </si>
+  <si>
+    <t>3.260</t>
+  </si>
+  <si>
+    <t>8.946</t>
+  </si>
+  <si>
+    <t>19.857</t>
+  </si>
+  <si>
+    <t>29.512</t>
+  </si>
+  <si>
+    <t>61.953</t>
+  </si>
+  <si>
+    <t>26.919</t>
+  </si>
+  <si>
+    <t>9287.121</t>
+  </si>
+  <si>
+    <t>27.623</t>
+  </si>
+  <si>
+    <t>0.214</t>
+  </si>
+  <si>
+    <t>0.633</t>
+  </si>
+  <si>
+    <t>3.630</t>
+  </si>
+  <si>
+    <t>9.168</t>
+  </si>
+  <si>
+    <t>17.597</t>
+  </si>
+  <si>
+    <t>24.198</t>
+  </si>
+  <si>
+    <t>45.837</t>
+  </si>
+  <si>
+    <t>38.517</t>
+  </si>
+  <si>
+    <t>12981.281</t>
+  </si>
+  <si>
+    <t>39.028</t>
+  </si>
+  <si>
+    <t>0.218</t>
+  </si>
+  <si>
+    <t>1.184</t>
+  </si>
+  <si>
+    <t>5.719</t>
+  </si>
+  <si>
+    <t>17.559</t>
+  </si>
+  <si>
+    <t>40.218</t>
+  </si>
+  <si>
+    <t>55.802</t>
+  </si>
+  <si>
+    <t>66.271</t>
+  </si>
+  <si>
+    <t>71.338</t>
+  </si>
+  <si>
+    <t>14017.971</t>
+  </si>
+  <si>
+    <t>71.872</t>
+  </si>
+  <si>
+    <t>20.000</t>
+  </si>
+  <si>
+    <t>1000000.000</t>
+  </si>
+  <si>
+    <t>0.365</t>
+  </si>
+  <si>
+    <t>0.667</t>
+  </si>
+  <si>
+    <t>4.185</t>
+  </si>
+  <si>
+    <t>10.978</t>
+  </si>
+  <si>
+    <t>26.129</t>
+  </si>
+  <si>
+    <t>63.318</t>
+  </si>
+  <si>
+    <t>76.290</t>
+  </si>
+  <si>
+    <t>44.273</t>
+  </si>
+  <si>
+    <t>5646.910</t>
+  </si>
+  <si>
+    <t>44.973</t>
+  </si>
+  <si>
+    <t>0.366</t>
+  </si>
+  <si>
+    <t>1.114</t>
+  </si>
+  <si>
+    <t>5.326</t>
+  </si>
+  <si>
+    <t>12.192</t>
+  </si>
+  <si>
+    <t>23.927</t>
+  </si>
+  <si>
+    <t>605.754</t>
+  </si>
+  <si>
+    <t>607.195</t>
+  </si>
+  <si>
+    <t>68.573</t>
+  </si>
+  <si>
+    <t>7291.500</t>
+  </si>
+  <si>
+    <t>69.139</t>
+  </si>
+  <si>
+    <t>Amazon EC2, m5.xlarge</t>
+  </si>
+  <si>
+    <t>60% CPU</t>
+  </si>
+  <si>
+    <t>70% CPU</t>
+  </si>
+  <si>
+    <t>0.367</t>
+  </si>
+  <si>
+    <t>2.090</t>
+  </si>
+  <si>
+    <t>9.166</t>
+  </si>
+  <si>
+    <t>18.972</t>
+  </si>
+  <si>
+    <t>49.683</t>
+  </si>
+  <si>
+    <t>865.960</t>
+  </si>
+  <si>
+    <t>874.300</t>
+  </si>
+  <si>
+    <t>125.385</t>
+  </si>
+  <si>
+    <t>7975.499</t>
+  </si>
+  <si>
+    <t>126.004</t>
+  </si>
+  <si>
+    <t>93% CPU</t>
+  </si>
+  <si>
+    <t>0.131</t>
+  </si>
+  <si>
+    <t>0.208</t>
+  </si>
+  <si>
+    <t>1.080</t>
+  </si>
+  <si>
+    <t>5.025</t>
+  </si>
+  <si>
+    <t>11.670</t>
+  </si>
+  <si>
+    <t>15.494</t>
+  </si>
+  <si>
+    <t>17.531</t>
+  </si>
+  <si>
+    <t>12.975</t>
+  </si>
+  <si>
+    <t>19267.823</t>
+  </si>
+  <si>
+    <t>13.990</t>
+  </si>
+  <si>
+    <t>0.130</t>
+  </si>
+  <si>
+    <t>0.260</t>
+  </si>
+  <si>
+    <t>1.563</t>
+  </si>
+  <si>
+    <t>8.009</t>
+  </si>
+  <si>
+    <t>16.059</t>
+  </si>
+  <si>
+    <t>27.739</t>
+  </si>
+  <si>
+    <t>39.314</t>
+  </si>
+  <si>
+    <t>18.206</t>
+  </si>
+  <si>
+    <t>27463.474</t>
+  </si>
+  <si>
+    <t>19.018</t>
+  </si>
+  <si>
+    <t>0.133</t>
+  </si>
+  <si>
+    <t>0.406</t>
+  </si>
+  <si>
+    <t>1.724</t>
+  </si>
+  <si>
+    <t>10.893</t>
+  </si>
+  <si>
+    <t>24.805</t>
+  </si>
+  <si>
+    <t>37.629</t>
+  </si>
+  <si>
+    <t>52.668</t>
+  </si>
+  <si>
+    <t>26.875</t>
+  </si>
+  <si>
+    <t>37209.302</t>
+  </si>
+  <si>
+    <t>27.646</t>
+  </si>
+  <si>
+    <t>0.129</t>
+  </si>
+  <si>
+    <t>0.784</t>
+  </si>
+  <si>
+    <t>3.449</t>
+  </si>
+  <si>
+    <t>14.095</t>
+  </si>
+  <si>
+    <t>29.663</t>
+  </si>
+  <si>
+    <t>59.085</t>
+  </si>
+  <si>
+    <t>70.397</t>
+  </si>
+  <si>
+    <t>45.874</t>
+  </si>
+  <si>
+    <t>43597.681</t>
+  </si>
+  <si>
+    <t>46.717</t>
+  </si>
+  <si>
+    <t>40.000</t>
+  </si>
+  <si>
+    <t>2000000.000</t>
+  </si>
+  <si>
+    <t>0.128</t>
+  </si>
+  <si>
+    <t>1.530</t>
+  </si>
+  <si>
+    <t>7.267</t>
+  </si>
+  <si>
+    <t>18.560</t>
+  </si>
+  <si>
+    <t>35.058</t>
+  </si>
+  <si>
+    <t>62.742</t>
+  </si>
+  <si>
+    <t>89.524</t>
+  </si>
+  <si>
+    <t>52.346</t>
+  </si>
+  <si>
+    <t>45848.775</t>
+  </si>
+  <si>
+    <t>53.414</t>
+  </si>
+  <si>
+    <t>80.000</t>
+  </si>
+  <si>
+    <t>2400000.000</t>
+  </si>
+  <si>
+    <t>0.201</t>
+  </si>
+  <si>
+    <t>0.345</t>
+  </si>
+  <si>
+    <t>2.349</t>
+  </si>
+  <si>
+    <t>9.665</t>
+  </si>
+  <si>
+    <t>22.421</t>
+  </si>
+  <si>
+    <t>138.627</t>
+  </si>
+  <si>
+    <t>141.747</t>
+  </si>
+  <si>
+    <t>23.804</t>
+  </si>
+  <si>
+    <t>10502.437</t>
+  </si>
+  <si>
+    <t>24.683</t>
+  </si>
+  <si>
+    <t>min=0,08 ms, avg=0.09 ms</t>
+  </si>
+  <si>
+    <t>0.187</t>
+  </si>
+  <si>
+    <t>0.467</t>
+  </si>
+  <si>
+    <t>1.715</t>
+  </si>
+  <si>
+    <t>10.317</t>
+  </si>
+  <si>
+    <t>16.760</t>
+  </si>
+  <si>
+    <t>28.941</t>
+  </si>
+  <si>
+    <t>31.265</t>
+  </si>
+  <si>
+    <t>29.963</t>
+  </si>
+  <si>
+    <t>16687.248</t>
+  </si>
+  <si>
+    <t>30.735</t>
+  </si>
+  <si>
+    <t>0.186</t>
+  </si>
+  <si>
+    <t>0.830</t>
+  </si>
+  <si>
+    <t>3.778</t>
+  </si>
+  <si>
+    <t>14.848</t>
+  </si>
+  <si>
+    <t>26.225</t>
+  </si>
+  <si>
+    <t>42.248</t>
+  </si>
+  <si>
+    <t>50.940</t>
+  </si>
+  <si>
+    <t>52.932</t>
+  </si>
+  <si>
+    <t>18892.520</t>
+  </si>
+  <si>
+    <t>53.697</t>
+  </si>
+  <si>
+    <t>50% CPU</t>
+  </si>
+  <si>
+    <t>78% CPU</t>
+  </si>
+  <si>
+    <t>Increate memory up to 10G!!</t>
+  </si>
+  <si>
+    <t>0.184</t>
+  </si>
+  <si>
+    <t>1.328</t>
+  </si>
+  <si>
+    <t>12.899</t>
+  </si>
+  <si>
+    <t>28.094</t>
+  </si>
+  <si>
+    <t>49.915</t>
+  </si>
+  <si>
+    <t>191.730</t>
+  </si>
+  <si>
+    <t>196.411</t>
+  </si>
+  <si>
+    <t>44.974</t>
+  </si>
+  <si>
+    <t>8894.028</t>
+  </si>
+  <si>
+    <t>46.618</t>
+  </si>
+  <si>
+    <t>20000.000</t>
+  </si>
+  <si>
+    <t>400000.000</t>
+  </si>
+  <si>
+    <t>Machine get lost !  :)</t>
   </si>
 </sst>
 </file>
@@ -146,7 +688,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,6 +701,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
@@ -185,7 +734,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -197,6 +746,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -477,15 +1029,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P42"/>
+  <dimension ref="A1:R113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="C105" sqref="C105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
     <col min="3" max="3" width="16.85546875" customWidth="1"/>
     <col min="4" max="4" width="9.28515625" customWidth="1"/>
     <col min="11" max="11" width="9.85546875" customWidth="1"/>
@@ -496,99 +1049,99 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="1" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="K7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="N7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="O7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="P7" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="N7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="P7" s="2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>47</v>
       </c>
       <c r="B8" t="s">
         <v>0</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E8">
         <v>0.77100000000000002</v>
@@ -623,13 +1176,13 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>47</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E9">
         <v>0.79700000000000004</v>
@@ -667,13 +1220,13 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>47</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E10">
         <v>1.3080000000000001</v>
@@ -711,13 +1264,13 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>47</v>
       </c>
       <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
         <v>9</v>
-      </c>
-      <c r="C11" t="s">
-        <v>12</v>
       </c>
       <c r="E11">
         <v>8.5259999999999998</v>
@@ -761,13 +1314,13 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="B14" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E14">
         <v>1.075</v>
@@ -805,13 +1358,13 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="B15" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E15">
         <v>1.0409999999999999</v>
@@ -849,13 +1402,13 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="B16" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E16">
         <v>1.0389999999999999</v>
@@ -893,13 +1446,13 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
         <v>9</v>
-      </c>
-      <c r="C17" t="s">
-        <v>12</v>
       </c>
       <c r="E17">
         <v>8.9160000000000004</v>
@@ -940,13 +1493,13 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B19" t="s">
         <v>0</v>
       </c>
       <c r="C19" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E19">
         <v>0.68</v>
@@ -982,13 +1535,13 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B20" t="s">
         <v>0</v>
       </c>
       <c r="C20" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E20">
         <v>0.75800000000000001</v>
@@ -1026,13 +1579,13 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B21" t="s">
         <v>0</v>
       </c>
       <c r="C21" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E21">
         <v>0.55900000000000005</v>
@@ -1070,13 +1623,13 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" t="s">
         <v>9</v>
-      </c>
-      <c r="C22" t="s">
-        <v>12</v>
       </c>
       <c r="E22">
         <v>9.4529999999999994</v>
@@ -1117,53 +1670,53 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B30" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C30" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D30" s="5">
         <v>0.52600000000000002</v>
@@ -1207,13 +1760,13 @@
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B31" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C31" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D31" s="5">
         <v>0.42799999999999999</v>
@@ -1257,13 +1810,13 @@
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B32" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C32" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D32">
         <v>0.40899999999999997</v>
@@ -1307,13 +1860,13 @@
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B33" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C33" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D33" s="5">
         <v>0.66</v>
@@ -1357,53 +1910,53 @@
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="B41" t="s">
         <v>0</v>
       </c>
       <c r="C41" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E41">
         <v>1.2849999999999999</v>
@@ -1441,13 +1994,13 @@
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="B42" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C42" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E42">
         <v>0.98899999999999999</v>
@@ -1481,6 +2034,1952 @@
       </c>
       <c r="P42">
         <v>50000</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" s="1" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="2"/>
+      <c r="B53" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H53" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I53" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J53" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K53" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L53" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M53" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="N53" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="O53" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="P53" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>29</v>
+      </c>
+      <c r="B54" t="s">
+        <v>7</v>
+      </c>
+      <c r="C54" t="s">
+        <v>25</v>
+      </c>
+      <c r="D54">
+        <v>0.65600000000000003</v>
+      </c>
+      <c r="E54">
+        <v>1.292</v>
+      </c>
+      <c r="F54">
+        <v>12.332000000000001</v>
+      </c>
+      <c r="G54">
+        <v>15.853999999999999</v>
+      </c>
+      <c r="H54">
+        <v>23.759</v>
+      </c>
+      <c r="I54">
+        <v>25.372</v>
+      </c>
+      <c r="J54">
+        <v>25.4</v>
+      </c>
+      <c r="K54">
+        <v>101.895</v>
+      </c>
+      <c r="L54">
+        <v>490.70600000000002</v>
+      </c>
+      <c r="M54">
+        <v>103.94499999999999</v>
+      </c>
+      <c r="N54">
+        <v>1</v>
+      </c>
+      <c r="O54">
+        <v>50000</v>
+      </c>
+      <c r="P54">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>29</v>
+      </c>
+      <c r="B55" t="s">
+        <v>7</v>
+      </c>
+      <c r="C55" t="s">
+        <v>25</v>
+      </c>
+      <c r="D55">
+        <v>0.63600000000000001</v>
+      </c>
+      <c r="E55">
+        <v>1.17</v>
+      </c>
+      <c r="F55">
+        <v>11.991</v>
+      </c>
+      <c r="G55">
+        <v>14.567</v>
+      </c>
+      <c r="H55">
+        <v>21.785</v>
+      </c>
+      <c r="I55">
+        <v>22.933</v>
+      </c>
+      <c r="J55">
+        <v>24.064</v>
+      </c>
+      <c r="K55">
+        <v>87.308000000000007</v>
+      </c>
+      <c r="L55">
+        <v>1145.384</v>
+      </c>
+      <c r="M55">
+        <v>89.278999999999996</v>
+      </c>
+      <c r="N55">
+        <v>2</v>
+      </c>
+      <c r="O55">
+        <v>50000</v>
+      </c>
+      <c r="P55">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>29</v>
+      </c>
+      <c r="B56" t="s">
+        <v>7</v>
+      </c>
+      <c r="C56" t="s">
+        <v>25</v>
+      </c>
+      <c r="D56">
+        <v>0.65500000000000003</v>
+      </c>
+      <c r="E56">
+        <v>2.6070000000000002</v>
+      </c>
+      <c r="F56">
+        <v>11.984</v>
+      </c>
+      <c r="G56">
+        <v>18.542000000000002</v>
+      </c>
+      <c r="H56">
+        <v>25.334</v>
+      </c>
+      <c r="I56">
+        <v>37.5</v>
+      </c>
+      <c r="J56">
+        <v>42.844999999999999</v>
+      </c>
+      <c r="K56">
+        <v>158.66399999999999</v>
+      </c>
+      <c r="L56">
+        <v>1575.6669999999999</v>
+      </c>
+      <c r="M56">
+        <v>160.827</v>
+      </c>
+      <c r="N56">
+        <v>5</v>
+      </c>
+      <c r="O56">
+        <v>50000</v>
+      </c>
+      <c r="P56">
+        <v>250000</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>29</v>
+      </c>
+      <c r="B57" t="s">
+        <v>7</v>
+      </c>
+      <c r="C57" t="s">
+        <v>25</v>
+      </c>
+      <c r="D57">
+        <v>0.66500000000000004</v>
+      </c>
+      <c r="E57">
+        <v>5.2249999999999996</v>
+      </c>
+      <c r="F57">
+        <v>15.263999999999999</v>
+      </c>
+      <c r="G57">
+        <v>33.771999999999998</v>
+      </c>
+      <c r="H57">
+        <v>45.801000000000002</v>
+      </c>
+      <c r="I57">
+        <v>61.531999999999996</v>
+      </c>
+      <c r="J57">
+        <v>106.121</v>
+      </c>
+      <c r="K57">
+        <v>175.994</v>
+      </c>
+      <c r="L57">
+        <v>1704.6130000000001</v>
+      </c>
+      <c r="M57">
+        <v>178.137</v>
+      </c>
+      <c r="N57">
+        <v>10</v>
+      </c>
+      <c r="O57">
+        <v>30000</v>
+      </c>
+      <c r="P57">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>29</v>
+      </c>
+      <c r="B58" t="s">
+        <v>7</v>
+      </c>
+      <c r="C58" t="s">
+        <v>25</v>
+      </c>
+      <c r="D58">
+        <v>0.68400000000000005</v>
+      </c>
+      <c r="E58">
+        <v>8.0329999999999995</v>
+      </c>
+      <c r="F58">
+        <v>20.92</v>
+      </c>
+      <c r="G58">
+        <v>48.347000000000001</v>
+      </c>
+      <c r="H58">
+        <v>75.59</v>
+      </c>
+      <c r="I58">
+        <v>99.843999999999994</v>
+      </c>
+      <c r="J58">
+        <v>112.976</v>
+      </c>
+      <c r="K58">
+        <v>90.23</v>
+      </c>
+      <c r="L58">
+        <v>1662.4179999999999</v>
+      </c>
+      <c r="M58">
+        <v>92.840999999999994</v>
+      </c>
+      <c r="N58">
+        <v>15</v>
+      </c>
+      <c r="O58">
+        <v>10000</v>
+      </c>
+      <c r="P58">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>26</v>
+      </c>
+      <c r="B61" t="s">
+        <v>7</v>
+      </c>
+      <c r="C61" t="s">
+        <v>25</v>
+      </c>
+      <c r="D61">
+        <v>0.53400000000000003</v>
+      </c>
+      <c r="E61">
+        <v>1.171</v>
+      </c>
+      <c r="F61">
+        <v>11.420999999999999</v>
+      </c>
+      <c r="G61">
+        <v>15.661</v>
+      </c>
+      <c r="H61">
+        <v>23.748000000000001</v>
+      </c>
+      <c r="I61">
+        <v>26.657</v>
+      </c>
+      <c r="J61">
+        <v>29.137</v>
+      </c>
+      <c r="K61">
+        <v>82.927999999999997</v>
+      </c>
+      <c r="L61">
+        <v>602.94000000000005</v>
+      </c>
+      <c r="M61">
+        <v>85.834000000000003</v>
+      </c>
+      <c r="N61">
+        <v>1</v>
+      </c>
+      <c r="O61">
+        <v>50000</v>
+      </c>
+      <c r="P61">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>26</v>
+      </c>
+      <c r="B62" t="s">
+        <v>7</v>
+      </c>
+      <c r="C62" t="s">
+        <v>25</v>
+      </c>
+      <c r="D62">
+        <v>0.443</v>
+      </c>
+      <c r="E62">
+        <v>1.1020000000000001</v>
+      </c>
+      <c r="F62">
+        <v>11.997999999999999</v>
+      </c>
+      <c r="G62">
+        <v>19.417999999999999</v>
+      </c>
+      <c r="H62">
+        <v>26.469000000000001</v>
+      </c>
+      <c r="I62">
+        <v>33.948</v>
+      </c>
+      <c r="J62">
+        <v>37.31</v>
+      </c>
+      <c r="K62">
+        <v>85.387</v>
+      </c>
+      <c r="L62">
+        <v>1171.152</v>
+      </c>
+      <c r="M62">
+        <v>88.28</v>
+      </c>
+      <c r="N62">
+        <v>2</v>
+      </c>
+      <c r="O62">
+        <v>50000</v>
+      </c>
+      <c r="P62">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>26</v>
+      </c>
+      <c r="B63" t="s">
+        <v>7</v>
+      </c>
+      <c r="C63" t="s">
+        <v>25</v>
+      </c>
+      <c r="D63">
+        <v>0.46500000000000002</v>
+      </c>
+      <c r="E63">
+        <v>1.4730000000000001</v>
+      </c>
+      <c r="F63">
+        <v>13.045999999999999</v>
+      </c>
+      <c r="G63">
+        <v>25.439</v>
+      </c>
+      <c r="H63">
+        <v>36.628999999999998</v>
+      </c>
+      <c r="I63">
+        <v>42.305999999999997</v>
+      </c>
+      <c r="J63">
+        <v>42.862000000000002</v>
+      </c>
+      <c r="K63">
+        <v>68.078000000000003</v>
+      </c>
+      <c r="L63">
+        <v>2203.3870000000002</v>
+      </c>
+      <c r="M63">
+        <v>71.06</v>
+      </c>
+      <c r="N63">
+        <v>5</v>
+      </c>
+      <c r="O63">
+        <v>30000</v>
+      </c>
+      <c r="P63">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>26</v>
+      </c>
+      <c r="B64" t="s">
+        <v>7</v>
+      </c>
+      <c r="C64" t="s">
+        <v>25</v>
+      </c>
+      <c r="D64">
+        <v>0.53200000000000003</v>
+      </c>
+      <c r="E64">
+        <v>2.7639999999999998</v>
+      </c>
+      <c r="F64">
+        <v>16.128</v>
+      </c>
+      <c r="G64">
+        <v>36.479999999999997</v>
+      </c>
+      <c r="H64">
+        <v>54.155000000000001</v>
+      </c>
+      <c r="I64">
+        <v>85.334999999999994</v>
+      </c>
+      <c r="J64">
+        <v>87.54</v>
+      </c>
+      <c r="K64">
+        <v>108.35</v>
+      </c>
+      <c r="L64">
+        <v>2768.8049999999998</v>
+      </c>
+      <c r="M64">
+        <v>111.925</v>
+      </c>
+      <c r="N64">
+        <v>10</v>
+      </c>
+      <c r="O64">
+        <v>30000</v>
+      </c>
+      <c r="P64">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>26</v>
+      </c>
+      <c r="B65" t="s">
+        <v>7</v>
+      </c>
+      <c r="C65" t="s">
+        <v>25</v>
+      </c>
+      <c r="D65">
+        <v>0.61899999999999999</v>
+      </c>
+      <c r="E65">
+        <v>3.6240000000000001</v>
+      </c>
+      <c r="F65">
+        <v>18.178000000000001</v>
+      </c>
+      <c r="G65">
+        <v>42.616999999999997</v>
+      </c>
+      <c r="H65">
+        <v>87.004000000000005</v>
+      </c>
+      <c r="I65">
+        <v>211.4</v>
+      </c>
+      <c r="J65">
+        <v>218.608</v>
+      </c>
+      <c r="K65">
+        <v>140.58099999999999</v>
+      </c>
+      <c r="L65">
+        <v>3201.0239999999999</v>
+      </c>
+      <c r="M65">
+        <v>144.06800000000001</v>
+      </c>
+      <c r="N65">
+        <v>15</v>
+      </c>
+      <c r="O65">
+        <v>30000</v>
+      </c>
+      <c r="P65">
+        <v>450000</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>26</v>
+      </c>
+      <c r="B66" t="s">
+        <v>7</v>
+      </c>
+      <c r="C66" t="s">
+        <v>25</v>
+      </c>
+      <c r="D66">
+        <v>0.91300000000000003</v>
+      </c>
+      <c r="E66">
+        <v>7.0380000000000003</v>
+      </c>
+      <c r="F66">
+        <v>31.454000000000001</v>
+      </c>
+      <c r="G66">
+        <v>96.944999999999993</v>
+      </c>
+      <c r="H66">
+        <v>155.11600000000001</v>
+      </c>
+      <c r="I66">
+        <v>179.97900000000001</v>
+      </c>
+      <c r="J66">
+        <v>196.27799999999999</v>
+      </c>
+      <c r="K66">
+        <v>88.111999999999995</v>
+      </c>
+      <c r="L66">
+        <v>3404.7579999999998</v>
+      </c>
+      <c r="M66">
+        <v>92.19</v>
+      </c>
+      <c r="N66">
+        <v>30</v>
+      </c>
+      <c r="O66">
+        <v>10000</v>
+      </c>
+      <c r="P66">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>26</v>
+      </c>
+      <c r="B67" t="s">
+        <v>7</v>
+      </c>
+      <c r="C67" t="s">
+        <v>25</v>
+      </c>
+      <c r="D67">
+        <v>1.2969999999999999</v>
+      </c>
+      <c r="E67">
+        <v>10.773</v>
+      </c>
+      <c r="F67">
+        <v>38.131</v>
+      </c>
+      <c r="G67">
+        <v>119.625</v>
+      </c>
+      <c r="H67">
+        <v>217.66499999999999</v>
+      </c>
+      <c r="I67">
+        <v>272.815</v>
+      </c>
+      <c r="J67">
+        <v>303.94799999999998</v>
+      </c>
+      <c r="K67">
+        <v>126.876</v>
+      </c>
+      <c r="L67">
+        <v>3940.8870000000002</v>
+      </c>
+      <c r="M67">
+        <v>133.291</v>
+      </c>
+      <c r="N67">
+        <v>50</v>
+      </c>
+      <c r="O67">
+        <v>10000</v>
+      </c>
+      <c r="P67">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>26</v>
+      </c>
+      <c r="B68" t="s">
+        <v>7</v>
+      </c>
+      <c r="C68" t="s">
+        <v>25</v>
+      </c>
+      <c r="D68">
+        <v>0.96099999999999997</v>
+      </c>
+      <c r="E68">
+        <v>17.193000000000001</v>
+      </c>
+      <c r="F68">
+        <v>43.807000000000002</v>
+      </c>
+      <c r="G68">
+        <v>69.397000000000006</v>
+      </c>
+      <c r="H68">
+        <v>165.70099999999999</v>
+      </c>
+      <c r="I68">
+        <v>245.387</v>
+      </c>
+      <c r="J68">
+        <v>245.721</v>
+      </c>
+      <c r="K68">
+        <v>193.39699999999999</v>
+      </c>
+      <c r="L68">
+        <v>3878.0529999999999</v>
+      </c>
+      <c r="M68">
+        <v>207.041</v>
+      </c>
+      <c r="N68">
+        <v>75</v>
+      </c>
+      <c r="O68">
+        <v>10000</v>
+      </c>
+      <c r="P68">
+        <v>750000</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>26</v>
+      </c>
+      <c r="B70" t="s">
+        <v>9</v>
+      </c>
+      <c r="C70" t="s">
+        <v>25</v>
+      </c>
+      <c r="D70">
+        <v>0.82099999999999995</v>
+      </c>
+      <c r="E70">
+        <v>4.0170000000000003</v>
+      </c>
+      <c r="F70">
+        <v>25.231000000000002</v>
+      </c>
+      <c r="G70">
+        <v>39.283999999999999</v>
+      </c>
+      <c r="H70">
+        <v>73.864999999999995</v>
+      </c>
+      <c r="I70">
+        <v>119.267</v>
+      </c>
+      <c r="J70">
+        <v>122.886</v>
+      </c>
+      <c r="K70">
+        <v>69.843999999999994</v>
+      </c>
+      <c r="L70">
+        <v>715.88099999999997</v>
+      </c>
+      <c r="M70">
+        <v>75.635000000000005</v>
+      </c>
+      <c r="N70">
+        <v>5</v>
+      </c>
+      <c r="O70">
+        <v>10000</v>
+      </c>
+      <c r="P70">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>26</v>
+      </c>
+      <c r="B71" t="s">
+        <v>9</v>
+      </c>
+      <c r="C71" t="s">
+        <v>25</v>
+      </c>
+      <c r="D71">
+        <v>1.004</v>
+      </c>
+      <c r="E71">
+        <v>4.8339999999999996</v>
+      </c>
+      <c r="F71">
+        <v>20.388000000000002</v>
+      </c>
+      <c r="G71">
+        <v>33.171999999999997</v>
+      </c>
+      <c r="H71">
+        <v>56.6</v>
+      </c>
+      <c r="I71">
+        <v>333.45600000000002</v>
+      </c>
+      <c r="J71">
+        <v>333.471</v>
+      </c>
+      <c r="K71">
+        <v>62.918999999999997</v>
+      </c>
+      <c r="L71">
+        <v>1589.37</v>
+      </c>
+      <c r="M71">
+        <v>69.233000000000004</v>
+      </c>
+      <c r="N71">
+        <v>10</v>
+      </c>
+      <c r="O71">
+        <v>10000</v>
+      </c>
+      <c r="P71">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>26</v>
+      </c>
+      <c r="B72" t="s">
+        <v>9</v>
+      </c>
+      <c r="C72" t="s">
+        <v>25</v>
+      </c>
+      <c r="D72">
+        <v>1.5620000000000001</v>
+      </c>
+      <c r="E72">
+        <v>13.71</v>
+      </c>
+      <c r="F72">
+        <v>36.954999999999998</v>
+      </c>
+      <c r="G72">
+        <v>52.534999999999997</v>
+      </c>
+      <c r="H72">
+        <v>373.10399999999998</v>
+      </c>
+      <c r="I72">
+        <v>406.40600000000001</v>
+      </c>
+      <c r="J72">
+        <v>406.59100000000001</v>
+      </c>
+      <c r="K72">
+        <v>158.15899999999999</v>
+      </c>
+      <c r="L72">
+        <v>1896.837</v>
+      </c>
+      <c r="M72">
+        <v>167.816</v>
+      </c>
+      <c r="N72">
+        <v>30</v>
+      </c>
+      <c r="O72">
+        <v>10000</v>
+      </c>
+      <c r="P72">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A74" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B74" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C74" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D74" s="8">
+        <v>1.609</v>
+      </c>
+      <c r="E74" s="8">
+        <v>7.8259999999999996</v>
+      </c>
+      <c r="F74" s="8">
+        <v>36.735999999999997</v>
+      </c>
+      <c r="G74" s="8">
+        <v>76.421999999999997</v>
+      </c>
+      <c r="H74" s="8">
+        <v>125.358</v>
+      </c>
+      <c r="I74" s="8">
+        <v>455.755</v>
+      </c>
+      <c r="J74" s="8">
+        <v>455.834</v>
+      </c>
+      <c r="K74" s="8">
+        <v>115.215</v>
+      </c>
+      <c r="L74" s="8">
+        <v>433.971</v>
+      </c>
+      <c r="M74" s="8">
+        <v>123.261</v>
+      </c>
+      <c r="N74" s="8">
+        <v>5</v>
+      </c>
+      <c r="O74" s="8">
+        <v>10000</v>
+      </c>
+      <c r="P74" s="8">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A75" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B75" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C75" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D75" s="8">
+        <v>1.1930000000000001</v>
+      </c>
+      <c r="E75" s="8">
+        <v>10.778</v>
+      </c>
+      <c r="F75" s="8">
+        <v>56.133000000000003</v>
+      </c>
+      <c r="G75" s="8">
+        <v>101.547</v>
+      </c>
+      <c r="H75" s="8">
+        <v>134.78899999999999</v>
+      </c>
+      <c r="I75" s="8">
+        <v>151.29300000000001</v>
+      </c>
+      <c r="J75" s="8">
+        <v>158.93600000000001</v>
+      </c>
+      <c r="K75" s="8">
+        <v>143.46199999999999</v>
+      </c>
+      <c r="L75" s="8">
+        <v>697.04899999999998</v>
+      </c>
+      <c r="M75" s="8">
+        <v>147.63800000000001</v>
+      </c>
+      <c r="N75" s="8">
+        <v>10</v>
+      </c>
+      <c r="O75" s="8">
+        <v>10000</v>
+      </c>
+      <c r="P75" s="8">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A76" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B76" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C76" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D76" s="8">
+        <v>1.147</v>
+      </c>
+      <c r="E76" s="8">
+        <v>22.103000000000002</v>
+      </c>
+      <c r="F76" s="8">
+        <v>167.49600000000001</v>
+      </c>
+      <c r="G76" s="8">
+        <v>233.4</v>
+      </c>
+      <c r="H76" s="8">
+        <v>1551.4690000000001</v>
+      </c>
+      <c r="I76" s="8">
+        <v>1686.99</v>
+      </c>
+      <c r="J76" s="8">
+        <v>1758.5360000000001</v>
+      </c>
+      <c r="K76" s="8">
+        <v>246.61699999999999</v>
+      </c>
+      <c r="L76" s="8">
+        <v>973.173</v>
+      </c>
+      <c r="M76" s="8">
+        <v>253.684</v>
+      </c>
+      <c r="N76" s="8">
+        <v>30</v>
+      </c>
+      <c r="O76" s="8">
+        <v>8000</v>
+      </c>
+      <c r="P76" s="8">
+        <v>240000</v>
+      </c>
+    </row>
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A80" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A81" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A82" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A83" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A84" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A85" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A86" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A87" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="90" spans="1:18" s="1" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="2"/>
+      <c r="B90" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F90" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G90" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H90" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I90" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J90" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K90" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L90" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M90" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="N90" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="O90" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="P90" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>29</v>
+      </c>
+      <c r="B92" t="s">
+        <v>7</v>
+      </c>
+      <c r="C92" t="s">
+        <v>25</v>
+      </c>
+      <c r="D92" t="s">
+        <v>51</v>
+      </c>
+      <c r="E92" t="s">
+        <v>52</v>
+      </c>
+      <c r="F92" t="s">
+        <v>53</v>
+      </c>
+      <c r="G92" t="s">
+        <v>54</v>
+      </c>
+      <c r="H92" t="s">
+        <v>55</v>
+      </c>
+      <c r="I92" t="s">
+        <v>56</v>
+      </c>
+      <c r="J92" t="s">
+        <v>57</v>
+      </c>
+      <c r="K92" t="s">
+        <v>58</v>
+      </c>
+      <c r="L92" t="s">
+        <v>59</v>
+      </c>
+      <c r="M92" t="s">
+        <v>60</v>
+      </c>
+      <c r="N92" t="s">
+        <v>37</v>
+      </c>
+      <c r="O92" t="s">
+        <v>36</v>
+      </c>
+      <c r="P92" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>29</v>
+      </c>
+      <c r="B93" t="s">
+        <v>7</v>
+      </c>
+      <c r="C93" t="s">
+        <v>25</v>
+      </c>
+      <c r="D93" t="s">
+        <v>61</v>
+      </c>
+      <c r="E93" t="s">
+        <v>62</v>
+      </c>
+      <c r="F93" t="s">
+        <v>63</v>
+      </c>
+      <c r="G93" t="s">
+        <v>64</v>
+      </c>
+      <c r="H93" t="s">
+        <v>65</v>
+      </c>
+      <c r="I93" t="s">
+        <v>66</v>
+      </c>
+      <c r="J93" t="s">
+        <v>67</v>
+      </c>
+      <c r="K93" t="s">
+        <v>68</v>
+      </c>
+      <c r="L93" t="s">
+        <v>69</v>
+      </c>
+      <c r="M93" t="s">
+        <v>70</v>
+      </c>
+      <c r="N93" t="s">
+        <v>39</v>
+      </c>
+      <c r="O93" t="s">
+        <v>36</v>
+      </c>
+      <c r="P93" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>29</v>
+      </c>
+      <c r="B94" t="s">
+        <v>7</v>
+      </c>
+      <c r="C94" t="s">
+        <v>25</v>
+      </c>
+      <c r="D94" t="s">
+        <v>71</v>
+      </c>
+      <c r="E94" t="s">
+        <v>72</v>
+      </c>
+      <c r="F94" t="s">
+        <v>73</v>
+      </c>
+      <c r="G94" t="s">
+        <v>74</v>
+      </c>
+      <c r="H94" t="s">
+        <v>75</v>
+      </c>
+      <c r="I94" t="s">
+        <v>76</v>
+      </c>
+      <c r="J94" t="s">
+        <v>77</v>
+      </c>
+      <c r="K94" t="s">
+        <v>78</v>
+      </c>
+      <c r="L94" t="s">
+        <v>79</v>
+      </c>
+      <c r="M94" t="s">
+        <v>80</v>
+      </c>
+      <c r="N94" t="s">
+        <v>81</v>
+      </c>
+      <c r="O94" t="s">
+        <v>36</v>
+      </c>
+      <c r="P94" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="96" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>29</v>
+      </c>
+      <c r="B96" t="s">
+        <v>9</v>
+      </c>
+      <c r="C96" t="s">
+        <v>25</v>
+      </c>
+      <c r="D96" t="s">
+        <v>83</v>
+      </c>
+      <c r="E96" t="s">
+        <v>84</v>
+      </c>
+      <c r="F96" t="s">
+        <v>85</v>
+      </c>
+      <c r="G96" t="s">
+        <v>86</v>
+      </c>
+      <c r="H96" t="s">
+        <v>87</v>
+      </c>
+      <c r="I96" t="s">
+        <v>88</v>
+      </c>
+      <c r="J96" t="s">
+        <v>89</v>
+      </c>
+      <c r="K96" t="s">
+        <v>90</v>
+      </c>
+      <c r="L96" t="s">
+        <v>91</v>
+      </c>
+      <c r="M96" t="s">
+        <v>92</v>
+      </c>
+      <c r="N96" t="s">
+        <v>37</v>
+      </c>
+      <c r="O96" t="s">
+        <v>36</v>
+      </c>
+      <c r="P96" t="s">
+        <v>38</v>
+      </c>
+      <c r="R96" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="97" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>29</v>
+      </c>
+      <c r="B97" t="s">
+        <v>9</v>
+      </c>
+      <c r="C97" t="s">
+        <v>25</v>
+      </c>
+      <c r="D97" t="s">
+        <v>93</v>
+      </c>
+      <c r="E97" t="s">
+        <v>94</v>
+      </c>
+      <c r="F97" t="s">
+        <v>95</v>
+      </c>
+      <c r="G97" t="s">
+        <v>96</v>
+      </c>
+      <c r="H97" t="s">
+        <v>97</v>
+      </c>
+      <c r="I97" t="s">
+        <v>98</v>
+      </c>
+      <c r="J97" t="s">
+        <v>99</v>
+      </c>
+      <c r="K97" t="s">
+        <v>100</v>
+      </c>
+      <c r="L97" t="s">
+        <v>101</v>
+      </c>
+      <c r="M97" t="s">
+        <v>102</v>
+      </c>
+      <c r="N97" t="s">
+        <v>39</v>
+      </c>
+      <c r="O97" t="s">
+        <v>36</v>
+      </c>
+      <c r="P97" t="s">
+        <v>41</v>
+      </c>
+      <c r="R97" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="98" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>29</v>
+      </c>
+      <c r="B98" t="s">
+        <v>9</v>
+      </c>
+      <c r="C98" t="s">
+        <v>25</v>
+      </c>
+      <c r="D98" t="s">
+        <v>106</v>
+      </c>
+      <c r="E98" t="s">
+        <v>107</v>
+      </c>
+      <c r="F98" t="s">
+        <v>108</v>
+      </c>
+      <c r="G98" t="s">
+        <v>109</v>
+      </c>
+      <c r="H98" t="s">
+        <v>110</v>
+      </c>
+      <c r="I98" t="s">
+        <v>111</v>
+      </c>
+      <c r="J98" t="s">
+        <v>112</v>
+      </c>
+      <c r="K98" t="s">
+        <v>113</v>
+      </c>
+      <c r="L98" t="s">
+        <v>114</v>
+      </c>
+      <c r="M98" t="s">
+        <v>115</v>
+      </c>
+      <c r="N98" t="s">
+        <v>81</v>
+      </c>
+      <c r="O98" t="s">
+        <v>36</v>
+      </c>
+      <c r="P98" t="s">
+        <v>82</v>
+      </c>
+      <c r="R98" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="100" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>26</v>
+      </c>
+      <c r="B100" t="s">
+        <v>7</v>
+      </c>
+      <c r="C100" t="s">
+        <v>25</v>
+      </c>
+      <c r="D100" t="s">
+        <v>117</v>
+      </c>
+      <c r="E100" t="s">
+        <v>118</v>
+      </c>
+      <c r="F100" t="s">
+        <v>119</v>
+      </c>
+      <c r="G100" t="s">
+        <v>120</v>
+      </c>
+      <c r="H100" t="s">
+        <v>121</v>
+      </c>
+      <c r="I100" t="s">
+        <v>122</v>
+      </c>
+      <c r="J100" t="s">
+        <v>123</v>
+      </c>
+      <c r="K100" t="s">
+        <v>124</v>
+      </c>
+      <c r="L100" t="s">
+        <v>125</v>
+      </c>
+      <c r="M100" t="s">
+        <v>126</v>
+      </c>
+      <c r="N100" t="s">
+        <v>37</v>
+      </c>
+      <c r="O100" t="s">
+        <v>36</v>
+      </c>
+      <c r="P100" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="101" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>26</v>
+      </c>
+      <c r="B101" t="s">
+        <v>7</v>
+      </c>
+      <c r="C101" t="s">
+        <v>25</v>
+      </c>
+      <c r="D101" t="s">
+        <v>127</v>
+      </c>
+      <c r="E101" t="s">
+        <v>128</v>
+      </c>
+      <c r="F101" t="s">
+        <v>129</v>
+      </c>
+      <c r="G101" t="s">
+        <v>130</v>
+      </c>
+      <c r="H101" t="s">
+        <v>131</v>
+      </c>
+      <c r="I101" t="s">
+        <v>132</v>
+      </c>
+      <c r="J101" t="s">
+        <v>133</v>
+      </c>
+      <c r="K101" t="s">
+        <v>134</v>
+      </c>
+      <c r="L101" t="s">
+        <v>135</v>
+      </c>
+      <c r="M101" t="s">
+        <v>136</v>
+      </c>
+      <c r="N101" t="s">
+        <v>39</v>
+      </c>
+      <c r="O101" t="s">
+        <v>36</v>
+      </c>
+      <c r="P101" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="102" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>26</v>
+      </c>
+      <c r="B102" t="s">
+        <v>7</v>
+      </c>
+      <c r="C102" t="s">
+        <v>25</v>
+      </c>
+      <c r="D102" t="s">
+        <v>137</v>
+      </c>
+      <c r="E102" t="s">
+        <v>138</v>
+      </c>
+      <c r="F102" t="s">
+        <v>139</v>
+      </c>
+      <c r="G102" t="s">
+        <v>140</v>
+      </c>
+      <c r="H102" t="s">
+        <v>141</v>
+      </c>
+      <c r="I102" t="s">
+        <v>142</v>
+      </c>
+      <c r="J102" t="s">
+        <v>143</v>
+      </c>
+      <c r="K102" t="s">
+        <v>144</v>
+      </c>
+      <c r="L102" t="s">
+        <v>145</v>
+      </c>
+      <c r="M102" t="s">
+        <v>146</v>
+      </c>
+      <c r="N102" t="s">
+        <v>81</v>
+      </c>
+      <c r="O102" t="s">
+        <v>36</v>
+      </c>
+      <c r="P102" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="103" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>26</v>
+      </c>
+      <c r="B103" t="s">
+        <v>7</v>
+      </c>
+      <c r="C103" t="s">
+        <v>25</v>
+      </c>
+      <c r="D103" t="s">
+        <v>147</v>
+      </c>
+      <c r="E103" t="s">
+        <v>148</v>
+      </c>
+      <c r="F103" t="s">
+        <v>149</v>
+      </c>
+      <c r="G103" t="s">
+        <v>150</v>
+      </c>
+      <c r="H103" t="s">
+        <v>151</v>
+      </c>
+      <c r="I103" t="s">
+        <v>152</v>
+      </c>
+      <c r="J103" t="s">
+        <v>153</v>
+      </c>
+      <c r="K103" t="s">
+        <v>154</v>
+      </c>
+      <c r="L103" t="s">
+        <v>155</v>
+      </c>
+      <c r="M103" t="s">
+        <v>156</v>
+      </c>
+      <c r="N103" t="s">
+        <v>157</v>
+      </c>
+      <c r="O103" t="s">
+        <v>36</v>
+      </c>
+      <c r="P103" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="104" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>26</v>
+      </c>
+      <c r="B104" t="s">
+        <v>7</v>
+      </c>
+      <c r="C104" t="s">
+        <v>25</v>
+      </c>
+      <c r="D104" t="s">
+        <v>159</v>
+      </c>
+      <c r="E104" t="s">
+        <v>160</v>
+      </c>
+      <c r="F104" t="s">
+        <v>161</v>
+      </c>
+      <c r="G104" t="s">
+        <v>162</v>
+      </c>
+      <c r="H104" t="s">
+        <v>163</v>
+      </c>
+      <c r="I104" t="s">
+        <v>164</v>
+      </c>
+      <c r="J104" t="s">
+        <v>165</v>
+      </c>
+      <c r="K104" t="s">
+        <v>166</v>
+      </c>
+      <c r="L104" t="s">
+        <v>167</v>
+      </c>
+      <c r="M104" t="s">
+        <v>168</v>
+      </c>
+      <c r="N104" t="s">
+        <v>169</v>
+      </c>
+      <c r="O104" t="s">
+        <v>40</v>
+      </c>
+      <c r="P104" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="106" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>26</v>
+      </c>
+      <c r="B106" t="s">
+        <v>9</v>
+      </c>
+      <c r="C106" t="s">
+        <v>25</v>
+      </c>
+      <c r="D106" t="s">
+        <v>171</v>
+      </c>
+      <c r="E106" t="s">
+        <v>172</v>
+      </c>
+      <c r="F106" t="s">
+        <v>173</v>
+      </c>
+      <c r="G106" t="s">
+        <v>174</v>
+      </c>
+      <c r="H106" t="s">
+        <v>175</v>
+      </c>
+      <c r="I106" t="s">
+        <v>176</v>
+      </c>
+      <c r="J106" t="s">
+        <v>177</v>
+      </c>
+      <c r="K106" t="s">
+        <v>178</v>
+      </c>
+      <c r="L106" t="s">
+        <v>179</v>
+      </c>
+      <c r="M106" t="s">
+        <v>180</v>
+      </c>
+      <c r="N106" t="s">
+        <v>37</v>
+      </c>
+      <c r="O106" t="s">
+        <v>36</v>
+      </c>
+      <c r="P106" t="s">
+        <v>38</v>
+      </c>
+      <c r="R106" s="9" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="107" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>26</v>
+      </c>
+      <c r="B107" t="s">
+        <v>9</v>
+      </c>
+      <c r="C107" t="s">
+        <v>25</v>
+      </c>
+      <c r="D107" t="s">
+        <v>182</v>
+      </c>
+      <c r="E107" t="s">
+        <v>183</v>
+      </c>
+      <c r="F107" t="s">
+        <v>184</v>
+      </c>
+      <c r="G107" t="s">
+        <v>185</v>
+      </c>
+      <c r="H107" t="s">
+        <v>186</v>
+      </c>
+      <c r="I107" t="s">
+        <v>187</v>
+      </c>
+      <c r="J107" t="s">
+        <v>188</v>
+      </c>
+      <c r="K107" t="s">
+        <v>189</v>
+      </c>
+      <c r="L107" t="s">
+        <v>190</v>
+      </c>
+      <c r="M107" t="s">
+        <v>191</v>
+      </c>
+      <c r="N107" t="s">
+        <v>39</v>
+      </c>
+      <c r="O107" t="s">
+        <v>36</v>
+      </c>
+      <c r="P107" t="s">
+        <v>41</v>
+      </c>
+      <c r="R107" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="108" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>26</v>
+      </c>
+      <c r="B108" t="s">
+        <v>9</v>
+      </c>
+      <c r="C108" t="s">
+        <v>25</v>
+      </c>
+      <c r="D108" t="s">
+        <v>192</v>
+      </c>
+      <c r="E108" t="s">
+        <v>193</v>
+      </c>
+      <c r="F108" t="s">
+        <v>194</v>
+      </c>
+      <c r="G108" t="s">
+        <v>195</v>
+      </c>
+      <c r="H108" t="s">
+        <v>196</v>
+      </c>
+      <c r="I108" t="s">
+        <v>197</v>
+      </c>
+      <c r="J108" t="s">
+        <v>198</v>
+      </c>
+      <c r="K108" t="s">
+        <v>199</v>
+      </c>
+      <c r="L108" t="s">
+        <v>200</v>
+      </c>
+      <c r="M108" t="s">
+        <v>201</v>
+      </c>
+      <c r="N108" t="s">
+        <v>81</v>
+      </c>
+      <c r="O108" t="s">
+        <v>36</v>
+      </c>
+      <c r="P108" t="s">
+        <v>82</v>
+      </c>
+      <c r="R108" s="7" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="111" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A111" s="7" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="112" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>26</v>
+      </c>
+      <c r="B112" t="s">
+        <v>9</v>
+      </c>
+      <c r="C112" t="s">
+        <v>25</v>
+      </c>
+      <c r="D112" t="s">
+        <v>205</v>
+      </c>
+      <c r="E112" t="s">
+        <v>206</v>
+      </c>
+      <c r="F112" t="s">
+        <v>207</v>
+      </c>
+      <c r="G112" t="s">
+        <v>208</v>
+      </c>
+      <c r="H112" t="s">
+        <v>209</v>
+      </c>
+      <c r="I112" t="s">
+        <v>210</v>
+      </c>
+      <c r="J112" t="s">
+        <v>211</v>
+      </c>
+      <c r="K112" t="s">
+        <v>212</v>
+      </c>
+      <c r="L112" t="s">
+        <v>213</v>
+      </c>
+      <c r="M112" t="s">
+        <v>214</v>
+      </c>
+      <c r="N112" t="s">
+        <v>81</v>
+      </c>
+      <c r="O112" t="s">
+        <v>215</v>
+      </c>
+      <c r="P112" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>217</v>
       </c>
     </row>
   </sheetData>

</xml_diff>